<commit_message>
Changes empty student excel sheet
</commit_message>
<xml_diff>
--- a/data/student.xlsx
+++ b/data/student.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GDP2\Codeword-GDPII\Documentation\Sample Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531382\Videos\Codeword-GDPII\Documentation\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D617DD6-1548-4C52-9A17-A3D9ADA4204D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{459926E6-AB72-4201-BE14-219883BB730B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{380793A7-BFC7-4BE3-8F72-6DA14EB4AA13}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>EmailKey</t>
   </si>
@@ -74,6 +74,15 @@
     <t>Girish Guntuku</t>
   </si>
   <si>
+    <t>s531499@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Saicharan Gurudu</t>
+  </si>
+  <si>
+    <t>s531500@nwmissouri.edu</t>
+  </si>
+  <si>
     <t>Sravya Kancharla</t>
   </si>
   <si>
@@ -153,27 +162,16 @@
   </si>
   <si>
     <t>Denise Case</t>
-  </si>
-  <si>
-    <t>s@nwmissouri.edu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -196,16 +194,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -518,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{571B4D73-A7A5-4BD8-95E9-C43A1B0899D3}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,121 +583,126 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
         <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
         <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
         <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
         <v>31</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
         <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
         <v>35</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
         <v>37</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
         <v>39</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B21" t="s">
         <v>41</v>
       </c>
-      <c r="B21" t="s">
-        <v>14</v>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1" xr:uid="{63A9E782-62F0-4B9D-80F4-B7E14BCF3833}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added remainign function in controller
</commit_message>
<xml_diff>
--- a/data/student.xlsx
+++ b/data/student.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531382\Videos\Codeword-GDPII\Documentation\Sample Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GDP2\Codeword-GDPII\Documentation\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{459926E6-AB72-4201-BE14-219883BB730B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D617DD6-1548-4C52-9A17-A3D9ADA4204D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{380793A7-BFC7-4BE3-8F72-6DA14EB4AA13}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>EmailKey</t>
   </si>
@@ -74,15 +74,6 @@
     <t>Girish Guntuku</t>
   </si>
   <si>
-    <t>s531499@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Saicharan Gurudu</t>
-  </si>
-  <si>
-    <t>s531500@nwmissouri.edu</t>
-  </si>
-  <si>
     <t>Sravya Kancharla</t>
   </si>
   <si>
@@ -162,16 +153,27 @@
   </si>
   <si>
     <t>Denise Case</t>
+  </si>
+  <si>
+    <t>s@nwmissouri.edu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -194,13 +196,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -513,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{571B4D73-A7A5-4BD8-95E9-C43A1B0899D3}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,126 +588,121 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>40</v>
+      <c r="A21" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A21" r:id="rId1" xr:uid="{63A9E782-62F0-4B9D-80F4-B7E14BCF3833}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed issue in course validation
</commit_message>
<xml_diff>
--- a/data/student.xlsx
+++ b/data/student.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S530742\Desktop\CI\Codeword-GDPII\Documentation\Sample Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531384\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7367F85-0A97-47C2-A0B2-BC850921B020}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6645" xr2:uid="{D0B14EB6-2760-4452-AF9A-AAB23E3746F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,138 +30,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
-  <si>
-    <t>EmailKey</t>
-  </si>
-  <si>
-    <t>Fullname</t>
-  </si>
-  <si>
-    <t>s531519@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Yashwanth Reddy Bommineni</t>
-  </si>
-  <si>
-    <t>s530742@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Naveen Kumar Chandaluri</t>
-  </si>
-  <si>
-    <t>s531495@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Chaithanya Cherukuru</t>
-  </si>
-  <si>
-    <t>s531367@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Sai Sirisha Devineni</t>
-  </si>
-  <si>
-    <t>s531496@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Shivani Reddy Dodla</t>
-  </si>
-  <si>
-    <t>s531369@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Girish Guntuku</t>
-  </si>
-  <si>
-    <t>Sravya Kancharla</t>
-  </si>
-  <si>
-    <t>s531372@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Anurag Kumar</t>
-  </si>
-  <si>
-    <t>s530473@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Ujjawal Kumar</t>
-  </si>
-  <si>
-    <t>s531439@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Dattu Bhargav Medarametla</t>
-  </si>
-  <si>
-    <t>s531503@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Santosh Sekhar Muchkur Bogarajula</t>
-  </si>
-  <si>
-    <t>s531373@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Naveenkumar Nuggu</t>
-  </si>
-  <si>
-    <t>s531507@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Vijay Kumar Tupakula</t>
-  </si>
-  <si>
-    <t>s531508@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Satya Sai Ram Vankina</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t xml:space="preserve">email </t>
+  </si>
+  <si>
+    <t>s531384@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username </t>
+  </si>
+  <si>
+    <t>Srimai Reddy Yanala</t>
+  </si>
+  <si>
+    <t>srimai Reddy yanala</t>
+  </si>
+  <si>
+    <t>s531383@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vyshnavi </t>
   </si>
   <si>
     <t>s531382@nwmissouri.edu</t>
   </si>
   <si>
-    <t>Sreelekha Vijaya</t>
-  </si>
-  <si>
-    <t>mwoolery@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Matthew Woolery</t>
-  </si>
-  <si>
-    <t>s531383@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Vyshnavi Yalamareddy</t>
-  </si>
-  <si>
-    <t>s531384@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Srimai Reddy Yanala</t>
-  </si>
-  <si>
-    <t>hoot@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Charles Hoot</t>
-  </si>
-  <si>
-    <t>dcase@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Denise Case</t>
-  </si>
-  <si>
-    <t>s@nwmissouri.edu</t>
+    <t>sreelekha</t>
+  </si>
+  <si>
+    <t>sravya</t>
+  </si>
+  <si>
+    <t>s531396@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>s531381@nwmissouri.edu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -516,17 +427,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA91B052-542C-40C1-9209-2EC74EC968F8}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -534,182 +445,57 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
+      <c r="A2" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{C806D9CF-CCD7-4DD7-95A5-E5FB44614F5F}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{188D883D-0130-4DA3-A64C-9E03D829670A}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{A8EBE8FB-AF83-478C-A81D-B48E2FF3C9E4}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{5C72418C-1D3A-4AC3-9820-DD984C522946}"/>
+    <hyperlink ref="A3" r:id="rId5" display="s531384@nwmissouri.edu" xr:uid="{FA3FDC5D-B8B7-4341-908F-6B6B24823FA6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fetching json student data using api call
</commit_message>
<xml_diff>
--- a/data/student.xlsx
+++ b/data/student.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531384\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531500\Desktop\gdp2\Codeword-GDPII\Documentation\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7367F85-0A97-47C2-A0B2-BC850921B020}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21248B99-6418-4F26-9ABA-41692D618E79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6645" xr2:uid="{D0B14EB6-2760-4452-AF9A-AAB23E3746F5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,42 +30,132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t xml:space="preserve">email </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+  <si>
+    <t>EmailKey</t>
+  </si>
+  <si>
+    <t>Fullname</t>
+  </si>
+  <si>
+    <t>s531519@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Yashwanth Reddy Bommineni</t>
+  </si>
+  <si>
+    <t>s530742@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Naveen Kumar Chandaluri</t>
+  </si>
+  <si>
+    <t>s531495@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Chaithanya Cherukuru</t>
+  </si>
+  <si>
+    <t>s531367@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Sai Sirisha Devineni</t>
+  </si>
+  <si>
+    <t>s531496@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Shivani Reddy Dodla</t>
+  </si>
+  <si>
+    <t>s531369@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Girish Guntuku</t>
+  </si>
+  <si>
+    <t>Sravya Kancharla</t>
+  </si>
+  <si>
+    <t>s531372@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Anurag Kumar</t>
+  </si>
+  <si>
+    <t>s530473@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Ujjawal Kumar</t>
+  </si>
+  <si>
+    <t>s531439@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Dattu Bhargav Medarametla</t>
+  </si>
+  <si>
+    <t>s531503@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Santosh Sekhar Muchkur Bogarajula</t>
+  </si>
+  <si>
+    <t>s531373@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Naveenkumar Nuggu</t>
+  </si>
+  <si>
+    <t>s531507@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Vijay Kumar Tupakula</t>
+  </si>
+  <si>
+    <t>s531508@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Satya Sai Ram Vankina</t>
+  </si>
+  <si>
+    <t>s531382@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Sreelekha Vijaya</t>
+  </si>
+  <si>
+    <t>mwoolery@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Matthew Woolery</t>
+  </si>
+  <si>
+    <t>s531383@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Vyshnavi Yalamareddy</t>
   </si>
   <si>
     <t>s531384@nwmissouri.edu</t>
   </si>
   <si>
-    <t xml:space="preserve">Username </t>
-  </si>
-  <si>
     <t>Srimai Reddy Yanala</t>
   </si>
   <si>
-    <t>srimai Reddy yanala</t>
-  </si>
-  <si>
-    <t>s531383@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vyshnavi </t>
-  </si>
-  <si>
-    <t>s531382@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>sreelekha</t>
-  </si>
-  <si>
-    <t>sravya</t>
-  </si>
-  <si>
-    <t>s531396@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>s531381@nwmissouri.edu</t>
+    <t>hoot@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Charles Hoot</t>
+  </si>
+  <si>
+    <t>dcase@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Denise Case</t>
+  </si>
+  <si>
+    <t>s@nwmissouri.edu</t>
   </si>
 </sst>
 </file>
@@ -427,17 +517,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA91B052-542C-40C1-9209-2EC74EC968F8}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -445,57 +535,174 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{C806D9CF-CCD7-4DD7-95A5-E5FB44614F5F}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{188D883D-0130-4DA3-A64C-9E03D829670A}"/>
-    <hyperlink ref="A5" r:id="rId3" xr:uid="{A8EBE8FB-AF83-478C-A81D-B48E2FF3C9E4}"/>
-    <hyperlink ref="A6" r:id="rId4" xr:uid="{5C72418C-1D3A-4AC3-9820-DD984C522946}"/>
-    <hyperlink ref="A3" r:id="rId5" display="s531384@nwmissouri.edu" xr:uid="{FA3FDC5D-B8B7-4341-908F-6B6B24823FA6}"/>
+    <hyperlink ref="A21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed table in course student
</commit_message>
<xml_diff>
--- a/data/student.xlsx
+++ b/data/student.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531500\Desktop\gdp2\Codeword-GDPII\Documentation\Sample Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531382\Videos\Codeword-GDPII\Documentation\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21248B99-6418-4F26-9ABA-41692D618E79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{459926E6-AB72-4201-BE14-219883BB730B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{380793A7-BFC7-4BE3-8F72-6DA14EB4AA13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>EmailKey</t>
   </si>
@@ -74,6 +74,15 @@
     <t>Girish Guntuku</t>
   </si>
   <si>
+    <t>s531499@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t>Saicharan Gurudu</t>
+  </si>
+  <si>
+    <t>s531500@nwmissouri.edu</t>
+  </si>
+  <si>
     <t>Sravya Kancharla</t>
   </si>
   <si>
@@ -153,27 +162,16 @@
   </si>
   <si>
     <t>Denise Case</t>
-  </si>
-  <si>
-    <t>s@nwmissouri.edu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -196,16 +194,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -517,11 +512,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{571B4D73-A7A5-4BD8-95E9-C43A1B0899D3}">
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,121 +583,126 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
         <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
         <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
         <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
         <v>31</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
         <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
         <v>35</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
         <v>37</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
         <v>39</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B21" t="s">
         <v>41</v>
       </c>
-      <c r="B21" t="s">
-        <v>14</v>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixses issues on instructor dashboard
</commit_message>
<xml_diff>
--- a/data/student.xlsx
+++ b/data/student.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GDP II\Codeword-GDPII\Documentation\Sample Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531500\Desktop\gdp2\Codeword-GDPII\Documentation\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0BD67B-D938-4BBF-A3C6-C4889418610F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21248B99-6418-4F26-9ABA-41692D618E79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,6 +56,9 @@
     <t>Chaithanya Cherukuru</t>
   </si>
   <si>
+    <t>s531367@nwmissouri.edu</t>
+  </si>
+  <si>
     <t>Sai Sirisha Devineni</t>
   </si>
   <si>
@@ -153,9 +156,6 @@
   </si>
   <si>
     <t>s@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>s531367asdfnwmissouri.edu</t>
   </si>
 </sst>
 </file>
@@ -520,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,138 +564,138 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>